<commit_message>
Updated argument structure, issue log.
</commit_message>
<xml_diff>
--- a/doc/assurance/ZoneAlertService/5-Issues/issues.xlsx
+++ b/doc/assurance/ZoneAlertService/5-Issues/issues.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dependable/Contracts/ASTRA/Deliverables/OpenUxAS-ZoneAlert/doc/assurance/ZoneWarningService/5-Issues/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dependable/Contracts/ASTRA/Deliverables/OpenUxAS-ZoneAlert/doc/assurance/ZoneAlertService/5-Issues/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490F5E86-81D5-BE4C-941C-68958EF8EC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D92F7D6-A252-354A-944C-A62C82C73453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="500" windowWidth="33760" windowHeight="20740" xr2:uid="{C9A58872-7F3C-C947-8C7B-D579EDD417B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="64">
   <si>
     <t>Status</t>
   </si>
@@ -203,6 +203,33 @@
   </si>
   <si>
     <t>1.3 and 1.4 are resolved, therefore this issue is resolved.</t>
+  </si>
+  <si>
+    <t>CANCELED</t>
+  </si>
+  <si>
+    <t>Overall assurance argument form is too generic / abstract. The argument should directly represent the specific reasoning for the problem at hand and its solution.</t>
+  </si>
+  <si>
+    <t>Recording the initial problem, discussion with stakeholder</t>
+  </si>
+  <si>
+    <t>Attempt top rewrite the problem branch argument to be more specific</t>
+  </si>
+  <si>
+    <t>Review of rewrite with stakeholder, recording of comments</t>
+  </si>
+  <si>
+    <t>Hybrid argument with confidence wing. Such that the direct argument is the problem diagram</t>
+  </si>
+  <si>
+    <t>Problem diagram syntax is too nebulous and content needs to be made more accurate and complete, emblamatic.</t>
+  </si>
+  <si>
+    <t>Process and artifact evidence for problem argument is mostly not yet implemented. Build it</t>
+  </si>
+  <si>
+    <t>A domain-specific diagram or form for explanation of the solution specification should be provided. Right now we just use a behavior definition document. Is that good enough</t>
   </si>
 </sst>
 </file>
@@ -347,9 +374,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -387,7 +414,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -493,7 +520,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -635,7 +662,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -643,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50891FDD-30FA-7E4F-8B50-3438F693C3DF}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1213,7 +1240,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <v>9</v>
       </c>
@@ -1223,8 +1250,123 @@
       <c r="C33" s="6" t="s">
         <v>51</v>
       </c>
+      <c r="E33" s="4">
+        <v>45321</v>
+      </c>
+      <c r="F33" s="9">
+        <v>45352</v>
+      </c>
+      <c r="G33" s="4">
+        <v>45352</v>
+      </c>
       <c r="H33" s="6" t="s">
         <v>52</v>
+      </c>
+      <c r="I33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A34" s="10">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="4">
+        <v>45321</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="4">
+        <v>45321</v>
+      </c>
+      <c r="I35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A36" s="10">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="4">
+        <v>45379</v>
+      </c>
+      <c r="G36" s="4">
+        <v>45379</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G37" s="4">
+        <v>45446</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G38" s="4">
+        <v>45447</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="G39" s="4">
+        <v>45447</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="G41" s="4">
+        <v>45447</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G42" s="4">
+        <v>45447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Updated problem definition assurance argument to transitino to problem graph file 2. Updated issues list for asks and current work status
</commit_message>
<xml_diff>
--- a/doc/assurance/ZoneAlertService/5-Issues/issues.xlsx
+++ b/doc/assurance/ZoneAlertService/5-Issues/issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dependable/Contracts/ASTRA/Deliverables/OpenUxAS-ZoneAlert/doc/assurance/ZoneAlertService/5-Issues/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D92F7D6-A252-354A-944C-A62C82C73453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1277DF-5D38-D44B-99E4-F8DCB79B2C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="500" windowWidth="33760" windowHeight="20740" xr2:uid="{C9A58872-7F3C-C947-8C7B-D579EDD417B1}"/>
   </bookViews>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50891FDD-30FA-7E4F-8B50-3438F693C3DF}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
1. Created a more accurate problem space document. Improved state model for problems in the diagram. 2. Created a new version of the problem identification sub-argument. This form "explicated" references the problem diagram but argues why the identified problem exists and was found in the diagram.
</commit_message>
<xml_diff>
--- a/doc/assurance/ZoneAlertService/5-Issues/issues.xlsx
+++ b/doc/assurance/ZoneAlertService/5-Issues/issues.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dependable/Contracts/ASTRA/Deliverables/OpenUxAS-ZoneAlert/doc/assurance/ZoneAlertService/5-Issues/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1277DF-5D38-D44B-99E4-F8DCB79B2C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9CB5A8-5187-9944-A087-65DCFC4E3845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="500" windowWidth="33760" windowHeight="20740" xr2:uid="{C9A58872-7F3C-C947-8C7B-D579EDD417B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>Status</t>
   </si>
@@ -229,7 +229,22 @@
     <t>Process and artifact evidence for problem argument is mostly not yet implemented. Build it</t>
   </si>
   <si>
-    <t>A domain-specific diagram or form for explanation of the solution specification should be provided. Right now we just use a behavior definition document. Is that good enough</t>
+    <t>A domain-specific diagram or form for explanation of the solution specification should be provided. Right now we just use a behavior definition document. Is that good enough?</t>
+  </si>
+  <si>
+    <t>Rebuild problem space diagram to be more accurate.</t>
+  </si>
+  <si>
+    <t>Applied a state-based model to the definition of each problem and showed how they are defined against requirements in various hierarchies of sub-solution.</t>
+  </si>
+  <si>
+    <t>A version of the argument that refers to the problem diagram and explains intermediate solutions and the identification of the specific lower-level problem to solve has been written</t>
+  </si>
+  <si>
+    <t>Discussion and comparison of the two problem arguent versions (one that refers to problemSpace.png, and another that cites it and explains the diagram reasoning.)</t>
+  </si>
+  <si>
+    <t>CANCELLED</t>
   </si>
 </sst>
 </file>
@@ -670,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50891FDD-30FA-7E4F-8B50-3438F693C3DF}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,7 +1260,7 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>51</v>
@@ -1364,9 +1379,42 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="G42" s="4">
-        <v>45447</v>
+        <v>45478</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="G43" s="4">
+        <v>45478</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="G44" s="4">
+        <v>45478</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="H45" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated problem definition (diagram) and supporting argument.
</commit_message>
<xml_diff>
--- a/doc/assurance/ZoneAlertService/5-Issues/issues.xlsx
+++ b/doc/assurance/ZoneAlertService/5-Issues/issues.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dependable/Contracts/ASTRA/Deliverables/OpenUxAS-ZoneAlert/doc/assurance/ZoneAlertService/5-Issues/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9CB5A8-5187-9944-A087-65DCFC4E3845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD86FC0C-F7CA-C64F-B813-B97440806F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="500" windowWidth="33760" windowHeight="20740" xr2:uid="{C9A58872-7F3C-C947-8C7B-D579EDD417B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>Status</t>
   </si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>CANCELLED</t>
+  </si>
+  <si>
+    <t>Updated problem diagram and argument based on Sean's feedback</t>
+  </si>
+  <si>
+    <t>Rewrite problem diagram and argument based on Sean's feedback</t>
+  </si>
+  <si>
+    <t>Process argument eliminated from problem argument in favor of direct reasoning</t>
   </si>
 </sst>
 </file>
@@ -685,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50891FDD-30FA-7E4F-8B50-3438F693C3DF}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1300,7 +1309,7 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>62</v>
@@ -1308,39 +1317,42 @@
       <c r="E35" s="4">
         <v>45321</v>
       </c>
+      <c r="F35" s="9">
+        <v>45494</v>
+      </c>
       <c r="I35" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A36" s="10">
+    <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G36" s="4">
+        <v>45494</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A37" s="10">
         <v>12</v>
       </c>
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E37" s="4">
         <v>45379</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G37" s="4">
         <v>45379</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H37" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="I36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="G37" s="4">
-        <v>45446</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="I37" t="s">
         <v>8</v>
@@ -1348,73 +1360,112 @@
     </row>
     <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="G38" s="4">
-        <v>45447</v>
+        <v>45446</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="G39" s="4">
         <v>45447</v>
       </c>
       <c r="H39" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="G40" s="4">
+        <v>45447</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="G41" s="4">
+      <c r="I40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="G42" s="4">
         <v>45447</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="H42" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="G42" s="4">
-        <v>45478</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="I42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="G43" s="4">
         <v>45478</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="G44" s="4">
         <v>45478</v>
       </c>
       <c r="H44" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="G45" s="4">
+        <v>45478</v>
+      </c>
+      <c r="H45" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="I44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="H45" s="6" t="s">
+      <c r="I45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="G46" s="4">
+        <v>45482</v>
+      </c>
+      <c r="H46" s="6" t="s">
         <v>67</v>
+      </c>
+      <c r="I46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G47" s="4">
+        <v>45483</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="G48" s="4">
+        <v>45494</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I48" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>